<commit_message>
update readme & requirements.txt
</commit_message>
<xml_diff>
--- a/scrape-results-2023-06-20.xlsx
+++ b/scrape-results-2023-06-20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -37,151 +37,142 @@
     <t>source</t>
   </si>
   <si>
-    <t>Samsung Galaxy S23 S23+ Plus 8/128 8/256 8/512 8GB 128GB 256GB SEIN</t>
-  </si>
-  <si>
-    <t>Rp12.199.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/9/8bd9f257-609c-4bdc-98bc-f24a070fac51.jpg</t>
-  </si>
-  <si>
-    <t>Original-Link</t>
-  </si>
-  <si>
-    <t>Jakarta Utara</t>
-  </si>
-  <si>
-    <t>Terjual 70+</t>
+    <t>(IBOX) Apple iPhone 14 512GB 256GB 128GB 6.1" inch Resmi Indo TAM</t>
+  </si>
+  <si>
+    <t>Rp13.580.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2022/10/21/f4c2f823-4297-4da7-a416-dd7658ccaf91.jpg</t>
+  </si>
+  <si>
+    <t>Putra Group</t>
+  </si>
+  <si>
+    <t>Jakarta Pusat</t>
+  </si>
+  <si>
+    <t>Terjual 100+</t>
   </si>
   <si>
     <t>Tokopedia</t>
   </si>
   <si>
-    <t>(RESMI) Samsung Galaxy S23 256GB 128GB Black Green Cream Lavender SEIN</t>
-  </si>
-  <si>
-    <t>Rp11.469.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/3/2/8e2b00a0-ee9d-4b36-b426-bea85eb343e8.jpg</t>
-  </si>
-  <si>
-    <t>Putra Group</t>
-  </si>
-  <si>
-    <t>Jakarta Pusat</t>
+    <t>iPhone 14 Promax Garansi Resmi</t>
+  </si>
+  <si>
+    <t>Rp29.000.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2022/12/17/deb74364-7a7a-44a7-a5db-b0ca4332dd8e.png</t>
+  </si>
+  <si>
+    <t>PT Pratama Sntra Semesta</t>
+  </si>
+  <si>
+    <t>Jakarta Barat</t>
+  </si>
+  <si>
+    <t>Terjual 500+</t>
+  </si>
+  <si>
+    <t>[PASTI RESMI] Apple iPhone 14 PRO MAX 1TB 512GB 256GB 128GB Resmi</t>
+  </si>
+  <si>
+    <t>Rp20.105.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/17/237017e6-ae9d-44bc-b4a9-a5a315ec563c.png</t>
+  </si>
+  <si>
+    <t>Apple Bank</t>
   </si>
   <si>
     <t>Terjual 30+</t>
   </si>
   <si>
-    <t>HP Samsung Galaxy S23 Ultra 12/256 12/512 GB 12/1TB 12GB 256GB SEIN</t>
-  </si>
-  <si>
-    <t>Rp17.825.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/5/15/a814edcf-3e96-423e-ae30-09bb17b05dd3.jpg</t>
-  </si>
-  <si>
-    <t>artic</t>
-  </si>
-  <si>
-    <t>Terjual 23</t>
-  </si>
-  <si>
-    <t>(RESMI) Samsung Galaxy S23 Ultra 1TB 512GB 256GB Black Green Cream Lav</t>
-  </si>
-  <si>
-    <t>Rp17.449.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/3/2/0ad7379e-bd62-40e9-8c75-1ba8d8e43c67.jpg</t>
-  </si>
-  <si>
-    <t>Terjual 90+</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 Ultra 12/256 12/512 12/1TB 12GB 256GB 512GB SEIN</t>
-  </si>
-  <si>
-    <t>Rp17.875.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/4/27/3c632ec7-ff86-49af-837a-1de58d238a48.jpg</t>
-  </si>
-  <si>
-    <t>Gallery Gadget Shop</t>
-  </si>
-  <si>
-    <t>Terjual 19</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 Plus S23+ / S23 5G 8/512GB 8/256GB Garansi Resmi</t>
-  </si>
-  <si>
-    <t>Rp13.999.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/6/20/870d4e90-4bee-413c-b897-ea814f7ee2ad.jpg</t>
-  </si>
-  <si>
-    <t>Dewa Ponsel Rakyat</t>
+    <t>RESMI iPhone 14 5G 128 / 256 / 512 Midnight Starlight Purple Blue - 128GB SINGLE, RED</t>
+  </si>
+  <si>
+    <t>Rp12.319.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2022/9/15/34d4b699-5a4a-46d6-9220-4593e02297a2.jpg</t>
+  </si>
+  <si>
+    <t>tokohapedia</t>
+  </si>
+  <si>
+    <t>Terjual 50+</t>
+  </si>
+  <si>
+    <t>Iphone 14 128 New garansi resmi blm aktif</t>
+  </si>
+  <si>
+    <t>Rp13.700.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/6/18/4d428a92-f853-4fb4-a207-963f7e90e3aa.jpg</t>
+  </si>
+  <si>
+    <t>Ilham Pusat HP Second BPP</t>
+  </si>
+  <si>
+    <t>Balikpapan</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Pro Garansi Resmi - 128GB 256GB 512GB 1TB</t>
+  </si>
+  <si>
+    <t>Rp17.269.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/4/6a115d00-bc7d-4d29-beb1-7939b44983f5.jpg</t>
+  </si>
+  <si>
+    <t>iSmile Official Store</t>
+  </si>
+  <si>
+    <t>Terjual 750+</t>
+  </si>
+  <si>
+    <t>iPhone 14 Garansi Resmi</t>
+  </si>
+  <si>
+    <t>Rp13.390.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/3/9/2cc67a4b-0bd9-4ae8-a35b-1d1bdec850ec.png</t>
   </si>
   <si>
     <t>Terjual 250+</t>
   </si>
   <si>
-    <t>Samsung Galaxy S23 Ultra 5G 12/1TB 12/512GB Garansi Resmi SEIN</t>
-  </si>
-  <si>
-    <t>Rp25.999.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/6/6/47923973-0519-487e-9ca6-022b4919b6ba.jpg</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 Ultra 5G Garansi Resmi SEIN</t>
-  </si>
-  <si>
-    <t>Rp18.765.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/3/14/35b8df86-1f54-4628-beb3-1070d4db5090.jpg</t>
-  </si>
-  <si>
-    <t>Senjaya Selindo</t>
-  </si>
-  <si>
-    <t>(RESMI) Samsung Galaxy S23 Ultra S23+ Plus S23 1TB 512GB 256GB 128GB</t>
-  </si>
-  <si>
-    <t>Rp11.499.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/2/6f162c8e-38d0-4e85-91f4-2018b47f4b0a.jpg</t>
-  </si>
-  <si>
-    <t>Terjual 500+</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 Ultra / S23 PLUS 5G 128GB 256GB 512GB 1Tb New Resmi</t>
-  </si>
-  <si>
-    <t>Rp11.200.000</t>
-  </si>
-  <si>
-    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/18/b3d117fd-f5b2-443b-bdcf-b503b4b3b737.jpg</t>
-  </si>
-  <si>
-    <t>EraZone</t>
-  </si>
-  <si>
-    <t>Jakarta Barat</t>
-  </si>
-  <si>
-    <t>Terjual 100+</t>
+    <t>iPhone 14 Pro Garansi Resmi</t>
+  </si>
+  <si>
+    <t>Rp17.910.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2022/12/17/fd8a942f-df0a-4c9a-9cef-014f16d32bc6.png</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Pro Max Garansi Resmi - 128GB 256GB 512GB 1TB Promax</t>
+  </si>
+  <si>
+    <t>Rp19.159.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/15/5e89831a-e8a9-4f20-af9c-c701c347d1c3.jpg</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Garansi Resmi - 128GB 256GB 512GB</t>
+  </si>
+  <si>
+    <t>Rp13.389.000</t>
+  </si>
+  <si>
+    <t>https://images.tokopedia.net/img/cache/200-square/VqbcmM/2023/2/15/0c4eabda-32af-4afa-b5b4-5a1363c705c4.jpg</t>
   </si>
 </sst>
 </file>
@@ -615,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -635,13 +626,13 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -649,22 +640,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -672,22 +660,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -695,22 +683,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -718,22 +706,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
@@ -741,22 +729,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -773,13 +761,13 @@
         <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>

</xml_diff>